<commit_message>
Change Ybus for hybrid ac/dc network
</commit_message>
<xml_diff>
--- a/Examples/paper_participation/ModalConfig.xlsx
+++ b/Examples/paper_participation/ModalConfig.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\paper_participation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE593EE0-EE71-46C5-8FED-4102BE605D24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEF93ED-575C-46B0-BC0E-FB80CD95137D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1013" yWindow="2737" windowWidth="3600" windowHeight="1846" firstSheet="2" activeTab="2" xr2:uid="{2B771158-C5EF-47E5-B0CD-8BA481E90AC5}"/>
   </bookViews>
   <sheets>
-    <sheet name="State-PF" sheetId="123" r:id="rId1"/>
-    <sheet name="Impedance-PF" sheetId="124" r:id="rId2"/>
-    <sheet name="Enabling" sheetId="125" r:id="rId3"/>
+    <sheet name="State-PF" sheetId="141" r:id="rId1"/>
+    <sheet name="Impedance-PF" sheetId="142" r:id="rId2"/>
+    <sheet name="Enabling" sheetId="143" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +92,7 @@
     <t>Mode5</t>
   </si>
   <si>
-    <t>-3745991.33+50.00i</t>
+    <t>-2494320.45+50.00i</t>
   </si>
   <si>
     <t>Device2</t>
@@ -101,31 +101,31 @@
     <t>Mode6</t>
   </si>
   <si>
-    <t>-3745991.33-50.00i</t>
+    <t>-2494320.45-50.00i</t>
   </si>
   <si>
     <t>Mode7</t>
   </si>
   <si>
-    <t>-2995548.71+50.00i</t>
+    <t>-230.40+135868.84i</t>
   </si>
   <si>
     <t>Mode8</t>
   </si>
   <si>
-    <t>-2995548.71-50.00i</t>
+    <t>-230.40-135868.84i</t>
   </si>
   <si>
     <t>Mode9</t>
   </si>
   <si>
-    <t>-2994991.60+50.00i</t>
+    <t>-230.40+135768.84i</t>
   </si>
   <si>
     <t>Mode10</t>
   </si>
   <si>
-    <t>-2994991.60-50.00i</t>
+    <t>-230.40-135768.84i</t>
   </si>
   <si>
     <t>Device3</t>
@@ -134,31 +134,31 @@
     <t>Mode11</t>
   </si>
   <si>
-    <t>-205226.64+50.00i</t>
+    <t>-18.65+119506.08i</t>
   </si>
   <si>
     <t>Mode12</t>
   </si>
   <si>
-    <t>-205226.64-50.00i</t>
+    <t>-18.65-119506.08i</t>
   </si>
   <si>
     <t>Mode13</t>
   </si>
   <si>
-    <t>-45264.64+49.99i</t>
+    <t>-18.65+119406.08i</t>
   </si>
   <si>
     <t>Mode14</t>
   </si>
   <si>
-    <t>-45264.64-49.99i</t>
+    <t>-18.65-119406.08i</t>
   </si>
   <si>
     <t>Mode15</t>
   </si>
   <si>
-    <t>-3821.95+50.00i</t>
+    <t>-29.14+98918.21i</t>
   </si>
   <si>
     <t>Device4</t>
@@ -167,19 +167,19 @@
     <t>Mode16</t>
   </si>
   <si>
-    <t>-3821.95-50.00i</t>
+    <t>-29.14-98918.21i</t>
   </si>
   <si>
     <t>Mode17</t>
   </si>
   <si>
-    <t>-4662.79+50.00i</t>
+    <t>-29.14+99018.21i</t>
   </si>
   <si>
     <t>Mode18</t>
   </si>
   <si>
-    <t>-4662.79-50.00i</t>
+    <t>-29.14-99018.21i</t>
   </si>
   <si>
     <t>i_d_i</t>
@@ -188,7 +188,7 @@
     <t>Mode19</t>
   </si>
   <si>
-    <t>-5029.52+50.00i</t>
+    <t>-5661.60+50.00i</t>
   </si>
   <si>
     <t>i_q_i</t>
@@ -197,7 +197,7 @@
     <t>Mode20</t>
   </si>
   <si>
-    <t>-5029.52-50.00i</t>
+    <t>-5661.60-50.00i</t>
   </si>
   <si>
     <t>w_pll_i</t>
@@ -209,13 +209,13 @@
     <t>Mode22</t>
   </si>
   <si>
-    <t>-26.06+99.72i</t>
+    <t>-25.78+100.29i</t>
   </si>
   <si>
     <t>Mode23</t>
   </si>
   <si>
-    <t>-26.06-99.72i</t>
+    <t>-25.78-100.29i</t>
   </si>
   <si>
     <t>v_dc</t>
@@ -224,7 +224,7 @@
     <t>Mode24</t>
   </si>
   <si>
-    <t>-3.99+53.56i</t>
+    <t>-3.14+54.10i</t>
   </si>
   <si>
     <t>v_dc_i</t>
@@ -233,7 +233,7 @@
     <t>Mode25</t>
   </si>
   <si>
-    <t>-3.99-53.56i</t>
+    <t>-3.14-54.10i</t>
   </si>
   <si>
     <t>Line</t>
@@ -245,7 +245,7 @@
     <t>Mode26</t>
   </si>
   <si>
-    <t>-5.55+50.00i</t>
+    <t>-5.56+50.00i</t>
   </si>
   <si>
     <t>x_br1-1_2</t>
@@ -254,7 +254,7 @@
     <t>Mode27</t>
   </si>
   <si>
-    <t>-5.55-50.00i</t>
+    <t>-5.56-50.00i</t>
   </si>
   <si>
     <t>x_br1-2_1</t>
@@ -263,7 +263,7 @@
     <t>Mode28</t>
   </si>
   <si>
-    <t>-5.64+50.04i</t>
+    <t>-5.65+50.04i</t>
   </si>
   <si>
     <t>x_br1-2_2</t>
@@ -272,7 +272,7 @@
     <t>Mode29</t>
   </si>
   <si>
-    <t>-5.64-50.04i</t>
+    <t>-5.65-50.04i</t>
   </si>
   <si>
     <t>x_br1-3_1</t>
@@ -287,25 +287,25 @@
     <t>Mode31</t>
   </si>
   <si>
-    <t>-0.16+8.14i</t>
+    <t>-0.08+8.13i</t>
   </si>
   <si>
     <t>Mode32</t>
   </si>
   <si>
-    <t>-0.16-8.14i</t>
+    <t>-0.08-8.13i</t>
   </si>
   <si>
     <t>Mode33</t>
   </si>
   <si>
-    <t>-7.02+4.77i</t>
+    <t>-6.99+4.77i</t>
   </si>
   <si>
     <t>Mode34</t>
   </si>
   <si>
-    <t>-7.02-4.77i</t>
+    <t>-6.99-4.77i</t>
   </si>
   <si>
     <t>Mode35</t>
@@ -314,13 +314,13 @@
     <t>Mode36</t>
   </si>
   <si>
-    <t>-0.01+3.06i</t>
+    <t>-0.00+3.01i</t>
   </si>
   <si>
     <t>Mode37</t>
   </si>
   <si>
-    <t>-0.01-3.06i</t>
+    <t>-0.00-3.01i</t>
   </si>
   <si>
     <t>Mode38</t>
@@ -846,7 +846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0AE263-6FF9-4DF3-9331-B7B99B1D3A68}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F2770F-57BE-486A-82C3-8018003F0B1B}">
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
@@ -1404,7 +1404,7 @@
         <v>80</v>
       </c>
       <c r="F36">
-        <v>-17.989999999999998</v>
+        <v>-17.899999999999999</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1489,7 +1489,7 @@
         <v>90</v>
       </c>
       <c r="F41">
-        <v>-6.51</v>
+        <v>-6.52</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1557,7 +1557,7 @@
         <v>96</v>
       </c>
       <c r="F45">
-        <v>-0.06</v>
+        <v>-0.04</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2012,7 +2012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57640E6F-629C-4EC9-985A-10B26D0F8704}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4C0978-5480-40BA-AB01-44CCE0201E98}">
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
@@ -2470,7 +2470,7 @@
         <v>80</v>
       </c>
       <c r="H37">
-        <v>-17.989999999999998</v>
+        <v>-17.899999999999999</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -2525,7 +2525,7 @@
         <v>90</v>
       </c>
       <c r="H42">
-        <v>-6.51</v>
+        <v>-6.52</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -2569,7 +2569,7 @@
         <v>96</v>
       </c>
       <c r="H46">
-        <v>-0.06</v>
+        <v>-0.04</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -2868,7 +2868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4BFC17-6186-4735-B951-BCF44AFB2BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7856D62-43A9-4197-94A9-8FAD2F59E807}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>